<commit_message>
fix: preencher header do relatorio de vendas por vendedor
</commit_message>
<xml_diff>
--- a/Output/Relatorio_DE767565.xlsx
+++ b/Output/Relatorio_DE767565.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\levi.sistemas\Downloads\NuCase\NubankCase_RelatorioVendas\Output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AEE3EF6-18BE-43E6-8408-CD266CD93EAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3073490C-3CC1-49A5-AB5D-EF58680182E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3540" yWindow="3540" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="{ID_VENDOR}" sheetId="1" r:id="rId1"/>
@@ -47,22 +47,7 @@
     <t>DATE</t>
   </si>
   <si>
-    <t>[D0]</t>
-  </si>
-  <si>
     <t>[Vendor Name]</t>
-  </si>
-  <si>
-    <t>[Street]</t>
-  </si>
-  <si>
-    <t>[District], [City], [State]</t>
-  </si>
-  <si>
-    <t>[Phone Number]</t>
-  </si>
-  <si>
-    <t>[e-Mail]</t>
   </si>
   <si>
     <t>INVOICE NUMBER / ITEM TYPE</t>
@@ -102,6 +87,21 @@
   </si>
   <si>
     <t>DE767565</t>
+  </si>
+  <si>
+    <t>07/29/2025</t>
+  </si>
+  <si>
+    <t>Avenida Senador Queirós lado par</t>
+  </si>
+  <si>
+    <t>Centro, São Paulo, SP</t>
+  </si>
+  <si>
+    <t>815-250-6051</t>
+  </si>
+  <si>
+    <t>tiger.shop@mail.com</t>
   </si>
 </sst>
 </file>
@@ -1086,10 +1086,10 @@
     <row r="7" spans="1:26" ht="30" customHeight="1">
       <c r="A7" s="3"/>
       <c r="B7" s="7" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="D7" s="8"/>
       <c r="E7" s="1"/>
@@ -1146,7 +1146,7 @@
     <row r="9" spans="1:26" ht="21.75" customHeight="1">
       <c r="A9" s="11"/>
       <c r="B9" s="12" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="13"/>
@@ -1176,7 +1176,7 @@
     <row r="10" spans="1:26" ht="25.5" customHeight="1">
       <c r="A10" s="11"/>
       <c r="B10" s="50" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="C10" s="45"/>
       <c r="D10" s="50"/>
@@ -1206,7 +1206,7 @@
     <row r="11" spans="1:26" ht="25.5" customHeight="1">
       <c r="A11" s="11"/>
       <c r="B11" s="15" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="15"/>
@@ -1236,7 +1236,7 @@
     <row r="12" spans="1:26" ht="25.5" customHeight="1">
       <c r="A12" s="11"/>
       <c r="B12" s="15" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="C12" s="6"/>
       <c r="D12" s="15"/>
@@ -1266,7 +1266,7 @@
     <row r="13" spans="1:26" ht="25.5" customHeight="1">
       <c r="A13" s="11"/>
       <c r="B13" s="15" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C13" s="6"/>
       <c r="D13" s="15"/>
@@ -1352,18 +1352,18 @@
     <row r="16" spans="1:26" ht="21" customHeight="1">
       <c r="A16" s="3"/>
       <c r="B16" s="51" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C16" s="52"/>
       <c r="D16" s="16" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E16" s="53" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="F16" s="52"/>
       <c r="G16" s="16" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="H16" s="10"/>
       <c r="I16" s="1"/>
@@ -1724,12 +1724,12 @@
     <row r="27" spans="1:26" ht="18.75" customHeight="1">
       <c r="A27" s="25"/>
       <c r="B27" s="26" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C27" s="27"/>
       <c r="D27" s="28"/>
       <c r="E27" s="29" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="F27" s="30"/>
       <c r="G27" s="31">
@@ -1765,7 +1765,7 @@
       <c r="C28" s="27"/>
       <c r="D28" s="28"/>
       <c r="E28" s="29" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F28" s="30"/>
       <c r="G28" s="31">
@@ -1797,7 +1797,7 @@
       <c r="C29" s="27"/>
       <c r="D29" s="28"/>
       <c r="E29" s="29" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="F29" s="30"/>
       <c r="G29" s="33">
@@ -1829,7 +1829,7 @@
       <c r="C30" s="27"/>
       <c r="D30" s="28"/>
       <c r="E30" s="29" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="F30" s="30"/>
       <c r="G30" s="31">
@@ -1862,7 +1862,7 @@
       <c r="C31" s="27"/>
       <c r="D31" s="28"/>
       <c r="E31" s="29" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="F31" s="30"/>
       <c r="G31" s="31">
@@ -1948,7 +1948,7 @@
     <row r="34" spans="1:26" ht="16.5" customHeight="1">
       <c r="A34" s="37"/>
       <c r="B34" s="5" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
@@ -1978,7 +1978,7 @@
     <row r="35" spans="1:26" ht="19.5" customHeight="1">
       <c r="A35" s="37"/>
       <c r="B35" s="58" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C35" s="45"/>
       <c r="D35" s="1"/>

</xml_diff>

<commit_message>
feat: escrevendo linhas das invoices com valores
</commit_message>
<xml_diff>
--- a/Output/Relatorio_DE767565.xlsx
+++ b/Output/Relatorio_DE767565.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\levi.sistemas\Downloads\NuCase\NubankCase_RelatorioVendas\Output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3073490C-3CC1-49A5-AB5D-EF58680182E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA7CD0B7-D708-49AE-A005-A2E96F8BC088}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>SALES REPORT</t>
   </si>
@@ -102,6 +102,9 @@
   </si>
   <si>
     <t>tiger.shop@mail.com</t>
+  </si>
+  <si>
+    <t>R$ 33689.27074150</t>
   </si>
 </sst>
 </file>
@@ -1415,7 +1418,9 @@
     </row>
     <row r="18" spans="1:26" ht="25.5" customHeight="1">
       <c r="A18" s="3"/>
-      <c r="B18" s="57"/>
+      <c r="B18" s="57" t="s">
+        <v>22</v>
+      </c>
       <c r="C18" s="56"/>
       <c r="D18" s="17">
         <v>0</v>

</xml_diff>

<commit_message>
feat: preenchendo corretamente linha de valores de invoice
</commit_message>
<xml_diff>
--- a/Output/Relatorio_DE767565.xlsx
+++ b/Output/Relatorio_DE767565.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\levi.sistemas\Downloads\NuCase\NubankCase_RelatorioVendas\Output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA7CD0B7-D708-49AE-A005-A2E96F8BC088}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F556893A-7C0E-4ECB-AD56-0696BF57CABC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -104,7 +104,7 @@
     <t>tiger.shop@mail.com</t>
   </si>
   <si>
-    <t>R$ 33689.27074150</t>
+    <t>663318 / Professional Services</t>
   </si>
 </sst>
 </file>
@@ -1423,15 +1423,15 @@
       </c>
       <c r="C18" s="56"/>
       <c r="D18" s="17">
-        <v>0</v>
+        <v>33704.92</v>
       </c>
       <c r="E18" s="55">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F18" s="56"/>
       <c r="G18" s="17">
         <f t="shared" ref="G18:G25" si="0">D18*E18</f>
-        <v>0</v>
+        <v>168524.59999999998</v>
       </c>
       <c r="H18" s="10"/>
       <c r="I18" s="1"/>
@@ -1739,7 +1739,7 @@
       <c r="F27" s="30"/>
       <c r="G27" s="31">
         <f>SUM(G18:G25)</f>
-        <v>0</v>
+        <v>168524.59999999998</v>
       </c>
       <c r="H27" s="32"/>
       <c r="I27" s="1"/>
@@ -1765,7 +1765,7 @@
       <c r="A28" s="25"/>
       <c r="B28" s="65">
         <f>G31</f>
-        <v>0</v>
+        <v>168524.59999999998</v>
       </c>
       <c r="C28" s="27"/>
       <c r="D28" s="28"/>
@@ -1872,7 +1872,7 @@
       <c r="F31" s="30"/>
       <c r="G31" s="31">
         <f>G27-G28+G30</f>
-        <v>0</v>
+        <v>168524.59999999998</v>
       </c>
       <c r="H31" s="32"/>
       <c r="I31" s="1"/>

</xml_diff>

<commit_message>
fix: correcao de leitura de subtotal
</commit_message>
<xml_diff>
--- a/Output/Relatorio_DE767565.xlsx
+++ b/Output/Relatorio_DE767565.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\levi.sistemas\Downloads\NuCase\NubankCase_RelatorioVendas\Output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F556893A-7C0E-4ECB-AD56-0696BF57CABC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1A7A62E-66CC-40DC-B771-C03472856980}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1423,7 +1423,7 @@
       </c>
       <c r="C18" s="56"/>
       <c r="D18" s="17">
-        <v>33704.92</v>
+        <v>33717.83</v>
       </c>
       <c r="E18" s="55">
         <v>5</v>
@@ -1431,7 +1431,7 @@
       <c r="F18" s="56"/>
       <c r="G18" s="17">
         <f t="shared" ref="G18:G25" si="0">D18*E18</f>
-        <v>168524.59999999998</v>
+        <v>168589.15000000002</v>
       </c>
       <c r="H18" s="10"/>
       <c r="I18" s="1"/>
@@ -1739,7 +1739,7 @@
       <c r="F27" s="30"/>
       <c r="G27" s="31">
         <f>SUM(G18:G25)</f>
-        <v>168524.59999999998</v>
+        <v>168589.15000000002</v>
       </c>
       <c r="H27" s="32"/>
       <c r="I27" s="1"/>
@@ -1765,7 +1765,7 @@
       <c r="A28" s="25"/>
       <c r="B28" s="65">
         <f>G31</f>
-        <v>168524.59999999998</v>
+        <v>910381.38000000012</v>
       </c>
       <c r="C28" s="27"/>
       <c r="D28" s="28"/>
@@ -1774,7 +1774,7 @@
       </c>
       <c r="F28" s="30"/>
       <c r="G28" s="31">
-        <v>0</v>
+        <v>16858.919999999998</v>
       </c>
       <c r="H28" s="32"/>
       <c r="I28" s="1"/>
@@ -1806,7 +1806,7 @@
       </c>
       <c r="F29" s="30"/>
       <c r="G29" s="33">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H29" s="32"/>
       <c r="I29" s="1"/>
@@ -1839,7 +1839,7 @@
       <c r="F30" s="30"/>
       <c r="G30" s="31">
         <f>(G27-G28)*G29</f>
-        <v>0</v>
+        <v>758651.15000000014</v>
       </c>
       <c r="H30" s="32"/>
       <c r="I30" s="1"/>
@@ -1872,7 +1872,7 @@
       <c r="F31" s="30"/>
       <c r="G31" s="31">
         <f>G27-G28+G30</f>
-        <v>168524.59999999998</v>
+        <v>910381.38000000012</v>
       </c>
       <c r="H31" s="32"/>
       <c r="I31" s="1"/>

</xml_diff>

<commit_message>
feat: feito rename sheet
</commit_message>
<xml_diff>
--- a/Output/Relatorio_DE767565.xlsx
+++ b/Output/Relatorio_DE767565.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\levi.sistemas\Downloads\NuCase\NubankCase_RelatorioVendas\Output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1A7A62E-66CC-40DC-B771-C03472856980}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05D76879-07C6-46FA-8662-2561DC19568B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="{ID_VENDOR}" sheetId="1" r:id="rId1"/>
+    <sheet name="DE767565" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1423,7 +1423,7 @@
       </c>
       <c r="C18" s="56"/>
       <c r="D18" s="17">
-        <v>33717.83</v>
+        <v>33689.89</v>
       </c>
       <c r="E18" s="55">
         <v>5</v>
@@ -1431,7 +1431,7 @@
       <c r="F18" s="56"/>
       <c r="G18" s="17">
         <f t="shared" ref="G18:G25" si="0">D18*E18</f>
-        <v>168589.15000000002</v>
+        <v>168449.45</v>
       </c>
       <c r="H18" s="10"/>
       <c r="I18" s="1"/>
@@ -1739,7 +1739,7 @@
       <c r="F27" s="30"/>
       <c r="G27" s="31">
         <f>SUM(G18:G25)</f>
-        <v>168589.15000000002</v>
+        <v>168449.45</v>
       </c>
       <c r="H27" s="32"/>
       <c r="I27" s="1"/>
@@ -1765,7 +1765,7 @@
       <c r="A28" s="25"/>
       <c r="B28" s="65">
         <f>G31</f>
-        <v>910381.38000000012</v>
+        <v>176871.92250000002</v>
       </c>
       <c r="C28" s="27"/>
       <c r="D28" s="28"/>
@@ -1774,7 +1774,7 @@
       </c>
       <c r="F28" s="30"/>
       <c r="G28" s="31">
-        <v>16858.919999999998</v>
+        <v>0</v>
       </c>
       <c r="H28" s="32"/>
       <c r="I28" s="1"/>
@@ -1806,7 +1806,7 @@
       </c>
       <c r="F29" s="30"/>
       <c r="G29" s="33">
-        <v>5</v>
+        <v>0.05</v>
       </c>
       <c r="H29" s="32"/>
       <c r="I29" s="1"/>
@@ -1839,7 +1839,7 @@
       <c r="F30" s="30"/>
       <c r="G30" s="31">
         <f>(G27-G28)*G29</f>
-        <v>758651.15000000014</v>
+        <v>8422.4725000000017</v>
       </c>
       <c r="H30" s="32"/>
       <c r="I30" s="1"/>
@@ -1872,7 +1872,7 @@
       <c r="F31" s="30"/>
       <c r="G31" s="31">
         <f>G27-G28+G30</f>
-        <v>910381.38000000012</v>
+        <v>176871.92250000002</v>
       </c>
       <c r="H31" s="32"/>
       <c r="I31" s="1"/>

</xml_diff>

<commit_message>
feat: gerando pdfs protegidos por senha
</commit_message>
<xml_diff>
--- a/Output/Relatorio_DE767565.xlsx
+++ b/Output/Relatorio_DE767565.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\levi.sistemas\Downloads\NuCase\NubankCase_RelatorioVendas\Output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05D76879-07C6-46FA-8662-2561DC19568B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38E4F7E3-49C0-47F5-BFF5-5CBD6FA03134}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1423,7 +1423,7 @@
       </c>
       <c r="C18" s="56"/>
       <c r="D18" s="17">
-        <v>33689.89</v>
+        <v>33734.58</v>
       </c>
       <c r="E18" s="55">
         <v>5</v>
@@ -1431,7 +1431,7 @@
       <c r="F18" s="56"/>
       <c r="G18" s="17">
         <f t="shared" ref="G18:G25" si="0">D18*E18</f>
-        <v>168449.45</v>
+        <v>168672.90000000002</v>
       </c>
       <c r="H18" s="10"/>
       <c r="I18" s="1"/>
@@ -1739,7 +1739,7 @@
       <c r="F27" s="30"/>
       <c r="G27" s="31">
         <f>SUM(G18:G25)</f>
-        <v>168449.45</v>
+        <v>168672.90000000002</v>
       </c>
       <c r="H27" s="32"/>
       <c r="I27" s="1"/>
@@ -1765,7 +1765,7 @@
       <c r="A28" s="25"/>
       <c r="B28" s="65">
         <f>G31</f>
-        <v>176871.92250000002</v>
+        <v>177106.54500000001</v>
       </c>
       <c r="C28" s="27"/>
       <c r="D28" s="28"/>
@@ -1839,7 +1839,7 @@
       <c r="F30" s="30"/>
       <c r="G30" s="31">
         <f>(G27-G28)*G29</f>
-        <v>8422.4725000000017</v>
+        <v>8433.6450000000023</v>
       </c>
       <c r="H30" s="32"/>
       <c r="I30" s="1"/>
@@ -1872,7 +1872,7 @@
       <c r="F31" s="30"/>
       <c r="G31" s="31">
         <f>G27-G28+G30</f>
-        <v>176871.92250000002</v>
+        <v>177106.54500000001</v>
       </c>
       <c r="H31" s="32"/>
       <c r="I31" s="1"/>

</xml_diff>

<commit_message>
fix: correcao do mes no texto do email, senha do pdf gerado, readme
</commit_message>
<xml_diff>
--- a/Output/Relatorio_DE767565.xlsx
+++ b/Output/Relatorio_DE767565.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\levi.sistemas\Downloads\NuCase\NubankCase_RelatorioVendas\Output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8103E0B1-22A4-4C9B-9394-3C82CF4F6830}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5214DEDB-DC8C-40E3-AF1D-7A77C16D1FE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,9 +45,6 @@
   </si>
   <si>
     <t>DATE</t>
-  </si>
-  <si>
-    <t>[Vendor Name]</t>
   </si>
   <si>
     <t>INVOICE NUMBER / ITEM TYPE</t>
@@ -96,6 +93,9 @@
   </si>
   <si>
     <t>Centro, São Paulo, SP</t>
+  </si>
+  <si>
+    <t>TIGER SHOP, INC</t>
   </si>
   <si>
     <t>815-250-6051</t>
@@ -1089,10 +1089,10 @@
     <row r="7" spans="1:26" ht="30" customHeight="1">
       <c r="A7" s="3"/>
       <c r="B7" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D7" s="8"/>
       <c r="E7" s="1"/>
@@ -1149,7 +1149,7 @@
     <row r="9" spans="1:26" ht="21.75" customHeight="1">
       <c r="A9" s="11"/>
       <c r="B9" s="12" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="13"/>
@@ -1179,7 +1179,7 @@
     <row r="10" spans="1:26" ht="25.5" customHeight="1">
       <c r="A10" s="11"/>
       <c r="B10" s="50" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C10" s="45"/>
       <c r="D10" s="50"/>
@@ -1209,7 +1209,7 @@
     <row r="11" spans="1:26" ht="25.5" customHeight="1">
       <c r="A11" s="11"/>
       <c r="B11" s="15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="15"/>
@@ -1355,18 +1355,18 @@
     <row r="16" spans="1:26" ht="21" customHeight="1">
       <c r="A16" s="3"/>
       <c r="B16" s="51" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C16" s="52"/>
       <c r="D16" s="16" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E16" s="53" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F16" s="52"/>
       <c r="G16" s="16" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H16" s="10"/>
       <c r="I16" s="1"/>
@@ -1423,7 +1423,7 @@
       </c>
       <c r="C18" s="56"/>
       <c r="D18" s="17">
-        <v>33781.32</v>
+        <v>33843.06</v>
       </c>
       <c r="E18" s="55">
         <v>5</v>
@@ -1431,7 +1431,7 @@
       <c r="F18" s="56"/>
       <c r="G18" s="17">
         <f t="shared" ref="G18:G25" si="0">D18*E18</f>
-        <v>168906.6</v>
+        <v>169215.3</v>
       </c>
       <c r="H18" s="10"/>
       <c r="I18" s="1"/>
@@ -1729,17 +1729,17 @@
     <row r="27" spans="1:26" ht="18.75" customHeight="1">
       <c r="A27" s="25"/>
       <c r="B27" s="26" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C27" s="27"/>
       <c r="D27" s="28"/>
       <c r="E27" s="29" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F27" s="30"/>
       <c r="G27" s="31">
         <f>SUM(G18:G25)</f>
-        <v>168906.6</v>
+        <v>169215.3</v>
       </c>
       <c r="H27" s="32"/>
       <c r="I27" s="1"/>
@@ -1765,12 +1765,12 @@
       <c r="A28" s="25"/>
       <c r="B28" s="65">
         <f>G31</f>
-        <v>177351.93</v>
+        <v>177676.065</v>
       </c>
       <c r="C28" s="27"/>
       <c r="D28" s="28"/>
       <c r="E28" s="29" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F28" s="30"/>
       <c r="G28" s="31">
@@ -1802,7 +1802,7 @@
       <c r="C29" s="27"/>
       <c r="D29" s="28"/>
       <c r="E29" s="29" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F29" s="30"/>
       <c r="G29" s="33">
@@ -1834,12 +1834,12 @@
       <c r="C30" s="27"/>
       <c r="D30" s="28"/>
       <c r="E30" s="29" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F30" s="30"/>
       <c r="G30" s="31">
         <f>(G27-G28)*G29</f>
-        <v>8445.33</v>
+        <v>8460.7649999999994</v>
       </c>
       <c r="H30" s="32"/>
       <c r="I30" s="1"/>
@@ -1867,12 +1867,12 @@
       <c r="C31" s="27"/>
       <c r="D31" s="28"/>
       <c r="E31" s="29" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F31" s="30"/>
       <c r="G31" s="31">
         <f>G27-G28+G30</f>
-        <v>177351.93</v>
+        <v>177676.065</v>
       </c>
       <c r="H31" s="32"/>
       <c r="I31" s="1"/>
@@ -1953,7 +1953,7 @@
     <row r="34" spans="1:26" ht="16.5" customHeight="1">
       <c r="A34" s="37"/>
       <c r="B34" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
@@ -1983,7 +1983,7 @@
     <row r="35" spans="1:26" ht="19.5" customHeight="1">
       <c r="A35" s="37"/>
       <c r="B35" s="58" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C35" s="45"/>
       <c r="D35" s="1"/>

</xml_diff>

<commit_message>
fix: correcao pdf pagians
</commit_message>
<xml_diff>
--- a/Output/Relatorio_DE767565.xlsx
+++ b/Output/Relatorio_DE767565.xlsx
@@ -2,13 +2,13 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
-  <workbookPr/>
+  <workbookPr codeName="EstaPastaDeTrabalho"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\levi.sistemas\Downloads\NuCase\NubankCase_RelatorioVendas\Output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8486ECE7-3142-44AD-9853-1459AB985E73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9E5CE1B-67BC-4CC8-AD71-821ABDE6EE24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -889,8 +889,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr>
+  <sheetPr codeName="Planilha1">
     <outlinePr summaryBelow="0" summaryRight="0"/>
+    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
@@ -1423,7 +1424,7 @@
       </c>
       <c r="C18" s="56"/>
       <c r="D18" s="17">
-        <v>33843.06</v>
+        <v>33806.99</v>
       </c>
       <c r="E18" s="55">
         <v>5</v>
@@ -1431,7 +1432,7 @@
       <c r="F18" s="56"/>
       <c r="G18" s="17">
         <f t="shared" ref="G18:G25" si="0">D18*E18</f>
-        <v>169215.3</v>
+        <v>169034.94999999998</v>
       </c>
       <c r="H18" s="10"/>
       <c r="I18" s="1"/>
@@ -1739,7 +1740,7 @@
       <c r="F27" s="30"/>
       <c r="G27" s="31">
         <f>SUM(G18:G25)</f>
-        <v>169215.3</v>
+        <v>169034.94999999998</v>
       </c>
       <c r="H27" s="32"/>
       <c r="I27" s="1"/>
@@ -1765,7 +1766,7 @@
       <c r="A28" s="25"/>
       <c r="B28" s="65">
         <f>G31</f>
-        <v>177676.065</v>
+        <v>177486.69749999998</v>
       </c>
       <c r="C28" s="27"/>
       <c r="D28" s="28"/>
@@ -1839,7 +1840,7 @@
       <c r="F30" s="30"/>
       <c r="G30" s="31">
         <f>(G27-G28)*G29</f>
-        <v>8460.7649999999994</v>
+        <v>8451.7474999999995</v>
       </c>
       <c r="H30" s="32"/>
       <c r="I30" s="1"/>
@@ -1872,7 +1873,7 @@
       <c r="F31" s="30"/>
       <c r="G31" s="31">
         <f>G27-G28+G30</f>
-        <v>177676.065</v>
+        <v>177486.69749999998</v>
       </c>
       <c r="H31" s="32"/>
       <c r="I31" s="1"/>
@@ -29059,8 +29060,8 @@
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="E16:F16"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="portrait"/>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0" footer="0"/>
+  <pageSetup fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix: separação do corpo enviado nos relatorios de erro
</commit_message>
<xml_diff>
--- a/Output/Relatorio_DE767565.xlsx
+++ b/Output/Relatorio_DE767565.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\levi.sistemas\Downloads\NuCase\NubankCase_RelatorioVendas\Output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D9BB65C-4187-4CB5-8FB0-A34A90B8E94E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AEAFAC4-B398-4178-8325-820B376B0F32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1374,7 +1374,7 @@
       </c>
       <c r="C18" s="35"/>
       <c r="D18" s="36">
-        <v>33798.42</v>
+        <v>33721.83</v>
       </c>
       <c r="E18" s="37">
         <v>5</v>
@@ -1382,7 +1382,7 @@
       <c r="F18" s="35"/>
       <c r="G18" s="36">
         <f t="shared" ref="G18:G25" si="0">D18*E18</f>
-        <v>168992.09999999998</v>
+        <v>168609.15000000002</v>
       </c>
       <c r="H18" s="23"/>
       <c r="I18" s="7"/>
@@ -1690,7 +1690,7 @@
       <c r="F27" s="3"/>
       <c r="G27" s="46">
         <f>SUM(G18:G25)</f>
-        <v>168992.09999999998</v>
+        <v>168609.15000000002</v>
       </c>
       <c r="H27" s="47"/>
       <c r="I27" s="7"/>
@@ -1716,7 +1716,7 @@
       <c r="A28" s="43"/>
       <c r="B28" s="48">
         <f>G31</f>
-        <v>177441.70499999999</v>
+        <v>177039.60750000001</v>
       </c>
       <c r="C28" s="44"/>
       <c r="D28" s="45"/>
@@ -1790,7 +1790,7 @@
       <c r="F30" s="3"/>
       <c r="G30" s="46">
         <f>(G27-G28)*G29</f>
-        <v>8449.6049999999996</v>
+        <v>8430.4575000000023</v>
       </c>
       <c r="H30" s="47"/>
       <c r="I30" s="7"/>
@@ -1823,7 +1823,7 @@
       <c r="F31" s="3"/>
       <c r="G31" s="46">
         <f>G27-G28+G30</f>
-        <v>177441.70499999999</v>
+        <v>177039.60750000001</v>
       </c>
       <c r="H31" s="47"/>
       <c r="I31" s="7"/>
@@ -28983,16 +28983,11 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="B35:C36"/>
-    <mergeCell ref="A38:H38"/>
-    <mergeCell ref="A39:E39"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="A1:H4"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="E16:F16"/>
     <mergeCell ref="C17:G17"/>
     <mergeCell ref="E18:F18"/>
     <mergeCell ref="E21:F21"/>
@@ -29004,11 +28999,16 @@
     <mergeCell ref="E20:F20"/>
     <mergeCell ref="B21:C21"/>
     <mergeCell ref="B22:C22"/>
-    <mergeCell ref="A1:H4"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="B35:C36"/>
+    <mergeCell ref="A38:H38"/>
+    <mergeCell ref="A39:E39"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="B28:B29"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0" footer="0"/>

</xml_diff>

<commit_message>
fix: logs de desconto
</commit_message>
<xml_diff>
--- a/Output/Relatorio_DE767565.xlsx
+++ b/Output/Relatorio_DE767565.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\levi.sistemas\Downloads\NuCase\NubankCase_RelatorioVendas\Output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AEAFAC4-B398-4178-8325-820B376B0F32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CD245EA-043D-4427-8FF5-72E9DA2A76C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1374,7 +1374,7 @@
       </c>
       <c r="C18" s="35"/>
       <c r="D18" s="36">
-        <v>33721.83</v>
+        <v>33687.550000000003</v>
       </c>
       <c r="E18" s="37">
         <v>5</v>
@@ -1382,7 +1382,7 @@
       <c r="F18" s="35"/>
       <c r="G18" s="36">
         <f t="shared" ref="G18:G25" si="0">D18*E18</f>
-        <v>168609.15000000002</v>
+        <v>168437.75</v>
       </c>
       <c r="H18" s="23"/>
       <c r="I18" s="7"/>
@@ -1690,7 +1690,7 @@
       <c r="F27" s="3"/>
       <c r="G27" s="46">
         <f>SUM(G18:G25)</f>
-        <v>168609.15000000002</v>
+        <v>168437.75</v>
       </c>
       <c r="H27" s="47"/>
       <c r="I27" s="7"/>
@@ -1716,7 +1716,7 @@
       <c r="A28" s="43"/>
       <c r="B28" s="48">
         <f>G31</f>
-        <v>177039.60750000001</v>
+        <v>176859.63750000001</v>
       </c>
       <c r="C28" s="44"/>
       <c r="D28" s="45"/>
@@ -1790,7 +1790,7 @@
       <c r="F30" s="3"/>
       <c r="G30" s="46">
         <f>(G27-G28)*G29</f>
-        <v>8430.4575000000023</v>
+        <v>8421.8875000000007</v>
       </c>
       <c r="H30" s="47"/>
       <c r="I30" s="7"/>
@@ -1823,7 +1823,7 @@
       <c r="F31" s="3"/>
       <c r="G31" s="46">
         <f>G27-G28+G30</f>
-        <v>177039.60750000001</v>
+        <v>176859.63750000001</v>
       </c>
       <c r="H31" s="47"/>
       <c r="I31" s="7"/>

</xml_diff>

<commit_message>
feat: adicionado anotações nos states para melhor compreensão.
</commit_message>
<xml_diff>
--- a/Output/Relatorio_DE767565.xlsx
+++ b/Output/Relatorio_DE767565.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\levi.sistemas\Downloads\NuCase\NubankCase_RelatorioVendas\Output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23767D25-22B7-4B77-89C7-5B3FE5CD7F84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4350C595-498B-43BE-B8D2-B3054896D531}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1374,7 +1374,7 @@
       </c>
       <c r="C18" s="35"/>
       <c r="D18" s="36">
-        <v>33692.28</v>
+        <v>33650.31</v>
       </c>
       <c r="E18" s="37">
         <v>5</v>
@@ -1382,7 +1382,7 @@
       <c r="F18" s="35"/>
       <c r="G18" s="36">
         <f t="shared" ref="G18:G25" si="0">D18*E18</f>
-        <v>168461.4</v>
+        <v>168251.55</v>
       </c>
       <c r="H18" s="23"/>
       <c r="I18" s="7"/>
@@ -1690,7 +1690,7 @@
       <c r="F27" s="3"/>
       <c r="G27" s="46">
         <f>SUM(G18:G25)</f>
-        <v>168461.4</v>
+        <v>168251.55</v>
       </c>
       <c r="H27" s="47"/>
       <c r="I27" s="7"/>
@@ -1716,7 +1716,7 @@
       <c r="A28" s="43"/>
       <c r="B28" s="48">
         <f>G31</f>
-        <v>176884.47</v>
+        <v>176664.1275</v>
       </c>
       <c r="C28" s="44"/>
       <c r="D28" s="45"/>
@@ -1790,7 +1790,7 @@
       <c r="F30" s="3"/>
       <c r="G30" s="46">
         <f>(G27-G28)*G29</f>
-        <v>8423.07</v>
+        <v>8412.5774999999994</v>
       </c>
       <c r="H30" s="47"/>
       <c r="I30" s="7"/>
@@ -1823,7 +1823,7 @@
       <c r="F31" s="3"/>
       <c r="G31" s="46">
         <f>G27-G28+G30</f>
-        <v>176884.47</v>
+        <v>176664.1275</v>
       </c>
       <c r="H31" s="47"/>
       <c r="I31" s="7"/>

</xml_diff>